<commit_message>
Impelmented all XOR instructions. Using new 3 step model for routing. Routing table->Instruction binding->Generalized instruction impelmentation
</commit_message>
<xml_diff>
--- a/Documents/OppCodes.xlsx
+++ b/Documents/OppCodes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthew\Documents\Gameboy emulator project\HazeEmu\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47F65533-F56A-4C31-832B-B585F8A33EEA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5E284E1-943F-4EE8-9614-6CD81AA9341F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="690" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2557,8 +2557,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:AJ50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R7" workbookViewId="0">
-      <selection activeCell="AA25" sqref="AA25"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="R33" sqref="R33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7463,6 +7463,37 @@
     </row>
   </sheetData>
   <mergeCells count="43">
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="T3:T5"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="T6:T8"/>
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="T9:T11"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="T12:T14"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="T15:T17"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="T18:T20"/>
+    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="T21:T23"/>
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="T24:T26"/>
+    <mergeCell ref="B27:B29"/>
+    <mergeCell ref="T27:T29"/>
+    <mergeCell ref="B30:B32"/>
+    <mergeCell ref="T30:T32"/>
+    <mergeCell ref="B33:B35"/>
+    <mergeCell ref="T33:T35"/>
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="T36:T38"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="T39:T41"/>
+    <mergeCell ref="B42:B44"/>
+    <mergeCell ref="F42:F44"/>
+    <mergeCell ref="N42:N44"/>
+    <mergeCell ref="P42:P44"/>
+    <mergeCell ref="T42:T44"/>
     <mergeCell ref="T45:T47"/>
     <mergeCell ref="B48:B50"/>
     <mergeCell ref="G48:G50"/>
@@ -7475,37 +7506,6 @@
     <mergeCell ref="N45:N47"/>
     <mergeCell ref="O45:O47"/>
     <mergeCell ref="P45:P47"/>
-    <mergeCell ref="B39:B41"/>
-    <mergeCell ref="T39:T41"/>
-    <mergeCell ref="B42:B44"/>
-    <mergeCell ref="F42:F44"/>
-    <mergeCell ref="N42:N44"/>
-    <mergeCell ref="P42:P44"/>
-    <mergeCell ref="T42:T44"/>
-    <mergeCell ref="B30:B32"/>
-    <mergeCell ref="T30:T32"/>
-    <mergeCell ref="B33:B35"/>
-    <mergeCell ref="T33:T35"/>
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="T36:T38"/>
-    <mergeCell ref="B21:B23"/>
-    <mergeCell ref="T21:T23"/>
-    <mergeCell ref="B24:B26"/>
-    <mergeCell ref="T24:T26"/>
-    <mergeCell ref="B27:B29"/>
-    <mergeCell ref="T27:T29"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="T12:T14"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="T15:T17"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="T18:T20"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="T3:T5"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="T6:T8"/>
-    <mergeCell ref="B9:B11"/>
-    <mergeCell ref="T9:T11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
@@ -12432,11 +12432,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="E3:E5"/>
-    <mergeCell ref="E6:E8"/>
-    <mergeCell ref="E9:E11"/>
-    <mergeCell ref="E21:E23"/>
-    <mergeCell ref="E24:E26"/>
     <mergeCell ref="E27:E29"/>
     <mergeCell ref="E12:E14"/>
     <mergeCell ref="E15:E17"/>
@@ -12448,6 +12443,11 @@
     <mergeCell ref="E30:E32"/>
     <mergeCell ref="E33:E35"/>
     <mergeCell ref="E36:E38"/>
+    <mergeCell ref="E3:E5"/>
+    <mergeCell ref="E6:E8"/>
+    <mergeCell ref="E9:E11"/>
+    <mergeCell ref="E21:E23"/>
+    <mergeCell ref="E24:E26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
@@ -17364,16 +17364,23 @@
     </row>
   </sheetData>
   <mergeCells count="43">
-    <mergeCell ref="T36:T38"/>
-    <mergeCell ref="T39:T41"/>
-    <mergeCell ref="T42:T44"/>
-    <mergeCell ref="T45:T47"/>
-    <mergeCell ref="T48:T50"/>
-    <mergeCell ref="T18:T20"/>
-    <mergeCell ref="T21:T23"/>
-    <mergeCell ref="T24:T26"/>
-    <mergeCell ref="T27:T29"/>
-    <mergeCell ref="T30:T32"/>
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="B27:B29"/>
+    <mergeCell ref="B30:B32"/>
+    <mergeCell ref="B33:B35"/>
+    <mergeCell ref="T3:T5"/>
+    <mergeCell ref="T6:T8"/>
+    <mergeCell ref="T9:T11"/>
+    <mergeCell ref="T12:T14"/>
+    <mergeCell ref="T15:T17"/>
     <mergeCell ref="T33:T35"/>
     <mergeCell ref="P45:P47"/>
     <mergeCell ref="B48:B50"/>
@@ -17390,23 +17397,16 @@
     <mergeCell ref="G45:G47"/>
     <mergeCell ref="N45:N47"/>
     <mergeCell ref="O45:O47"/>
-    <mergeCell ref="T3:T5"/>
-    <mergeCell ref="T6:T8"/>
-    <mergeCell ref="T9:T11"/>
-    <mergeCell ref="T12:T14"/>
-    <mergeCell ref="T15:T17"/>
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="B9:B11"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="B21:B23"/>
-    <mergeCell ref="B24:B26"/>
-    <mergeCell ref="B27:B29"/>
-    <mergeCell ref="B30:B32"/>
-    <mergeCell ref="B33:B35"/>
+    <mergeCell ref="T18:T20"/>
+    <mergeCell ref="T21:T23"/>
+    <mergeCell ref="T24:T26"/>
+    <mergeCell ref="T27:T29"/>
+    <mergeCell ref="T30:T32"/>
+    <mergeCell ref="T36:T38"/>
+    <mergeCell ref="T39:T41"/>
+    <mergeCell ref="T42:T44"/>
+    <mergeCell ref="T45:T47"/>
+    <mergeCell ref="T48:T50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>

<commit_message>
Implemented all increment and decrement instructions. Added support for CPU to obtain a reference to a memory location. This is used to allow values in memroy to be altered in-place. Am unable to properly test new additions. Next order of business will be to expand my options for interacting with the processor. I am planning to implement a launch argument that will start the processor in 'interactive mode'.
</commit_message>
<xml_diff>
--- a/Documents/OppCodes.xlsx
+++ b/Documents/OppCodes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthew\Documents\Gameboy emulator project\HazeEmu\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5E284E1-943F-4EE8-9614-6CD81AA9341F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7A6C1AA-320E-4D9C-9ADB-6C5BC215EDCC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="690" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2557,8 +2557,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:AJ50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="R33" sqref="R33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L37" sqref="L37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7463,37 +7463,6 @@
     </row>
   </sheetData>
   <mergeCells count="43">
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="T3:T5"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="T6:T8"/>
-    <mergeCell ref="B9:B11"/>
-    <mergeCell ref="T9:T11"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="T12:T14"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="T15:T17"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="T18:T20"/>
-    <mergeCell ref="B21:B23"/>
-    <mergeCell ref="T21:T23"/>
-    <mergeCell ref="B24:B26"/>
-    <mergeCell ref="T24:T26"/>
-    <mergeCell ref="B27:B29"/>
-    <mergeCell ref="T27:T29"/>
-    <mergeCell ref="B30:B32"/>
-    <mergeCell ref="T30:T32"/>
-    <mergeCell ref="B33:B35"/>
-    <mergeCell ref="T33:T35"/>
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="T36:T38"/>
-    <mergeCell ref="B39:B41"/>
-    <mergeCell ref="T39:T41"/>
-    <mergeCell ref="B42:B44"/>
-    <mergeCell ref="F42:F44"/>
-    <mergeCell ref="N42:N44"/>
-    <mergeCell ref="P42:P44"/>
-    <mergeCell ref="T42:T44"/>
     <mergeCell ref="T45:T47"/>
     <mergeCell ref="B48:B50"/>
     <mergeCell ref="G48:G50"/>
@@ -7506,6 +7475,37 @@
     <mergeCell ref="N45:N47"/>
     <mergeCell ref="O45:O47"/>
     <mergeCell ref="P45:P47"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="T39:T41"/>
+    <mergeCell ref="B42:B44"/>
+    <mergeCell ref="F42:F44"/>
+    <mergeCell ref="N42:N44"/>
+    <mergeCell ref="P42:P44"/>
+    <mergeCell ref="T42:T44"/>
+    <mergeCell ref="B30:B32"/>
+    <mergeCell ref="T30:T32"/>
+    <mergeCell ref="B33:B35"/>
+    <mergeCell ref="T33:T35"/>
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="T36:T38"/>
+    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="T21:T23"/>
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="T24:T26"/>
+    <mergeCell ref="B27:B29"/>
+    <mergeCell ref="T27:T29"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="T12:T14"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="T15:T17"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="T18:T20"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="T3:T5"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="T6:T8"/>
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="T9:T11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
@@ -12432,6 +12432,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="E3:E5"/>
+    <mergeCell ref="E6:E8"/>
+    <mergeCell ref="E9:E11"/>
+    <mergeCell ref="E21:E23"/>
+    <mergeCell ref="E24:E26"/>
     <mergeCell ref="E27:E29"/>
     <mergeCell ref="E12:E14"/>
     <mergeCell ref="E15:E17"/>
@@ -12443,11 +12448,6 @@
     <mergeCell ref="E30:E32"/>
     <mergeCell ref="E33:E35"/>
     <mergeCell ref="E36:E38"/>
-    <mergeCell ref="E3:E5"/>
-    <mergeCell ref="E6:E8"/>
-    <mergeCell ref="E9:E11"/>
-    <mergeCell ref="E21:E23"/>
-    <mergeCell ref="E24:E26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
@@ -17364,23 +17364,16 @@
     </row>
   </sheetData>
   <mergeCells count="43">
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="B9:B11"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="B21:B23"/>
-    <mergeCell ref="B24:B26"/>
-    <mergeCell ref="B27:B29"/>
-    <mergeCell ref="B30:B32"/>
-    <mergeCell ref="B33:B35"/>
-    <mergeCell ref="T3:T5"/>
-    <mergeCell ref="T6:T8"/>
-    <mergeCell ref="T9:T11"/>
-    <mergeCell ref="T12:T14"/>
-    <mergeCell ref="T15:T17"/>
+    <mergeCell ref="T36:T38"/>
+    <mergeCell ref="T39:T41"/>
+    <mergeCell ref="T42:T44"/>
+    <mergeCell ref="T45:T47"/>
+    <mergeCell ref="T48:T50"/>
+    <mergeCell ref="T18:T20"/>
+    <mergeCell ref="T21:T23"/>
+    <mergeCell ref="T24:T26"/>
+    <mergeCell ref="T27:T29"/>
+    <mergeCell ref="T30:T32"/>
     <mergeCell ref="T33:T35"/>
     <mergeCell ref="P45:P47"/>
     <mergeCell ref="B48:B50"/>
@@ -17397,16 +17390,23 @@
     <mergeCell ref="G45:G47"/>
     <mergeCell ref="N45:N47"/>
     <mergeCell ref="O45:O47"/>
-    <mergeCell ref="T18:T20"/>
-    <mergeCell ref="T21:T23"/>
-    <mergeCell ref="T24:T26"/>
-    <mergeCell ref="T27:T29"/>
-    <mergeCell ref="T30:T32"/>
-    <mergeCell ref="T36:T38"/>
-    <mergeCell ref="T39:T41"/>
-    <mergeCell ref="T42:T44"/>
-    <mergeCell ref="T45:T47"/>
-    <mergeCell ref="T48:T50"/>
+    <mergeCell ref="T3:T5"/>
+    <mergeCell ref="T6:T8"/>
+    <mergeCell ref="T9:T11"/>
+    <mergeCell ref="T12:T14"/>
+    <mergeCell ref="T15:T17"/>
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="B27:B29"/>
+    <mergeCell ref="B30:B32"/>
+    <mergeCell ref="B33:B35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>